<commit_message>
Add tumor extent columns.
</commit_message>
<xml_diff>
--- a/test/fixtures/qiprofile/breast/clinical.xlsx
+++ b/test/fixtures/qiprofile/breast/clinical.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="300" windowWidth="30520" windowHeight="18640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="200" yWindow="200" windowWidth="28140" windowHeight="14500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>Birth Date</t>
   </si>
@@ -272,8 +272,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -387,7 +389,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -426,6 +428,7 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -464,6 +467,7 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -884,7 +888,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR67"/>
+  <dimension ref="A1:AR68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1151,56 +1155,22 @@
     </row>
     <row r="5" spans="1:44" s="2" customFormat="1">
       <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>41661</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="2">
-        <v>48</v>
-      </c>
       <c r="G5" s="12">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H5" s="12">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I5" s="12">
-        <v>8</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>1</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="T5" s="2" t="s">
         <v>17</v>
@@ -1208,59 +1178,75 @@
       <c r="W5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Z5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:44" s="2" customFormat="1">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>41661</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="2">
+        <v>48</v>
+      </c>
+      <c r="G6" s="12">
+        <v>18</v>
+      </c>
+      <c r="H6" s="12">
+        <v>11</v>
+      </c>
+      <c r="I6" s="12">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB6" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:44">
-      <c r="A6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
-      <c r="AL6" s="2"/>
-      <c r="AM6" s="2"/>
-      <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
-      <c r="AP6" s="2"/>
-      <c r="AQ6" s="2"/>
-      <c r="AR6" s="2"/>
     </row>
     <row r="7" spans="1:44">
       <c r="A7" s="2"/>
@@ -1442,6 +1428,7 @@
       <c r="A11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -3889,21 +3876,64 @@
       <c r="AQ67" s="2"/>
       <c r="AR67" s="2"/>
     </row>
+    <row r="68" spans="1:44">
+      <c r="A68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2"/>
+      <c r="V68" s="2"/>
+      <c r="W68" s="2"/>
+      <c r="X68" s="2"/>
+      <c r="Y68" s="2"/>
+      <c r="Z68" s="2"/>
+      <c r="AA68" s="2"/>
+      <c r="AB68" s="2"/>
+      <c r="AC68" s="2"/>
+      <c r="AD68" s="2"/>
+      <c r="AE68" s="2"/>
+      <c r="AF68" s="2"/>
+      <c r="AG68" s="2"/>
+      <c r="AH68" s="2"/>
+      <c r="AI68" s="2"/>
+      <c r="AJ68" s="2"/>
+      <c r="AK68" s="2"/>
+      <c r="AL68" s="2"/>
+      <c r="AM68" s="2"/>
+      <c r="AN68" s="2"/>
+      <c r="AO68" s="2"/>
+      <c r="AP68" s="2"/>
+      <c r="AQ68" s="2"/>
+      <c r="AR68" s="2"/>
+    </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576 N2:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576 P2:P1048576">
       <formula1>"0,1,2,3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA1048576 O2:O1048576 R1:R1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1:R1048576 O2:O1048576 AA2:AA1048576">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q1048576 S2:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576 Q2:Q1048576">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W1048576 T2:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576 W2:W1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X1048576 U2:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576 X2:X1048576">
       <formula1>"0,1,2,3,4,5,6,7,8"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z1048576">

</xml_diff>

<commit_message>
Change node size column heading to node length.
</commit_message>
<xml_diff>
--- a/test/fixtures/qiprofile/breast/clinical.xlsx
+++ b/test/fixtures/qiprofile/breast/clinical.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="200" windowWidth="28140" windowHeight="14500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-25060" yWindow="720" windowWidth="20300" windowHeight="13300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Birth Date</t>
   </si>
@@ -202,6 +202,21 @@
   </si>
   <si>
     <t>Patient Weight (kg)</t>
+  </si>
+  <si>
+    <t>Tumor Cell Density</t>
+  </si>
+  <si>
+    <t>DCIS Cell Density</t>
+  </si>
+  <si>
+    <t>Positive Node Count</t>
+  </si>
+  <si>
+    <t>Total Node Count</t>
+  </si>
+  <si>
+    <t>Largest Nodal Metastasis Length (mm)</t>
   </si>
 </sst>
 </file>
@@ -272,8 +287,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -389,7 +420,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -429,6 +460,14 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -468,6 +507,14 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -888,10 +935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR68"/>
+  <dimension ref="A1:AW68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -899,12 +946,14 @@
     <col min="2" max="2" width="12" style="2"/>
     <col min="5" max="5" width="12.5" style="10" customWidth="1"/>
     <col min="7" max="9" width="12" style="13" customWidth="1"/>
-    <col min="10" max="11" width="12" customWidth="1"/>
-    <col min="12" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="20" width="12" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="12" width="12" style="13" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="25" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="5" customFormat="1" ht="45">
+    <row r="1" spans="1:49" s="5" customFormat="1" ht="60">
       <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
@@ -936,61 +985,76 @@
         <v>55</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:44" s="2" customFormat="1">
+    <row r="2" spans="1:49" s="2" customFormat="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1019,20 +1083,20 @@
       <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="12">
+        <v>60</v>
+      </c>
+      <c r="L2" s="12">
+        <v>30</v>
+      </c>
+      <c r="M2" s="2">
         <v>3</v>
-      </c>
-      <c r="L2" s="2">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2">
-        <v>2</v>
       </c>
       <c r="N2" s="2">
         <v>2</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>26</v>
+      <c r="O2" s="2">
+        <v>2</v>
       </c>
       <c r="P2" s="2">
         <v>2</v>
@@ -1040,41 +1104,56 @@
       <c r="Q2" s="2">
         <v>2</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="2">
+        <v>4</v>
+      </c>
+      <c r="S2" s="2">
+        <v>12</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="2">
+      <c r="U2" s="2">
+        <v>2</v>
+      </c>
+      <c r="V2" s="2">
+        <v>2</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="2">
         <v>1</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="2">
+      <c r="Z2" s="2">
         <v>5</v>
       </c>
-      <c r="V2" s="2">
+      <c r="AA2" s="2">
         <v>80</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="2">
+      <c r="AC2" s="2">
         <v>3</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="AD2" s="2">
         <v>40</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AG2" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:44" s="2" customFormat="1">
+    <row r="3" spans="1:49" s="2" customFormat="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1093,14 +1172,16 @@
       <c r="I3" s="12">
         <v>7</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="Y3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:44" s="2" customFormat="1">
+    <row r="4" spans="1:49" s="2" customFormat="1">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1131,29 +1212,44 @@
       <c r="J4" s="2">
         <v>2</v>
       </c>
-      <c r="K4" s="2">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
+      <c r="K4" s="12">
+        <v>40</v>
+      </c>
+      <c r="L4" s="12">
+        <v>10</v>
       </c>
       <c r="M4" s="2">
         <v>2</v>
       </c>
       <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
         <v>2</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2">
+        <v>2</v>
+      </c>
+      <c r="S4" s="2">
+        <v>8</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="2">
+      <c r="U4" s="2">
         <v>1</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="V4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:44" s="2" customFormat="1">
+    <row r="5" spans="1:49" s="2" customFormat="1">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1172,14 +1268,16 @@
       <c r="I5" s="12">
         <v>5</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="Y5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:44" s="2" customFormat="1">
+    <row r="6" spans="1:49" s="2" customFormat="1">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1208,47 +1306,60 @@
       <c r="J6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
+      <c r="K6" s="12">
+        <v>20</v>
+      </c>
+      <c r="L6" s="12"/>
       <c r="M6" s="2">
         <v>1</v>
       </c>
       <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1</v>
       </c>
       <c r="P6" s="2">
         <v>0</v>
       </c>
       <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
         <v>1</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="Y6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="AB6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AE6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AF6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AG6" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:49">
       <c r="A7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1257,8 +1368,8 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1291,8 +1402,13 @@
       <c r="AP7" s="2"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="2"/>
-    </row>
-    <row r="8" spans="1:44">
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+    </row>
+    <row r="8" spans="1:49">
       <c r="A8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1301,8 +1417,8 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1335,8 +1451,13 @@
       <c r="AP8" s="2"/>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
-    </row>
-    <row r="9" spans="1:44">
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+    </row>
+    <row r="9" spans="1:49">
       <c r="A9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1345,8 +1466,8 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1379,8 +1500,13 @@
       <c r="AP9" s="2"/>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2"/>
-    </row>
-    <row r="10" spans="1:44">
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+    </row>
+    <row r="10" spans="1:49">
       <c r="A10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1389,8 +1515,8 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1423,8 +1549,13 @@
       <c r="AP10" s="2"/>
       <c r="AQ10" s="2"/>
       <c r="AR10" s="2"/>
-    </row>
-    <row r="11" spans="1:44">
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+    </row>
+    <row r="11" spans="1:49">
       <c r="A11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1433,8 +1564,8 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1467,8 +1598,13 @@
       <c r="AP11" s="2"/>
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2"/>
-    </row>
-    <row r="12" spans="1:44">
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+    </row>
+    <row r="12" spans="1:49">
       <c r="A12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1476,8 +1612,8 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1510,8 +1646,13 @@
       <c r="AP12" s="2"/>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2"/>
-    </row>
-    <row r="13" spans="1:44">
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+    </row>
+    <row r="13" spans="1:49">
       <c r="A13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1519,8 +1660,8 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1553,8 +1694,13 @@
       <c r="AP13" s="2"/>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
-    </row>
-    <row r="14" spans="1:44">
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+    </row>
+    <row r="14" spans="1:49">
       <c r="A14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1562,8 +1708,8 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1596,8 +1742,13 @@
       <c r="AP14" s="2"/>
       <c r="AQ14" s="2"/>
       <c r="AR14" s="2"/>
-    </row>
-    <row r="15" spans="1:44">
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+    </row>
+    <row r="15" spans="1:49">
       <c r="A15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1605,8 +1756,8 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1639,8 +1790,13 @@
       <c r="AP15" s="2"/>
       <c r="AQ15" s="2"/>
       <c r="AR15" s="2"/>
-    </row>
-    <row r="16" spans="1:44">
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="AW15" s="2"/>
+    </row>
+    <row r="16" spans="1:49">
       <c r="A16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1648,8 +1804,8 @@
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1682,8 +1838,13 @@
       <c r="AP16" s="2"/>
       <c r="AQ16" s="2"/>
       <c r="AR16" s="2"/>
-    </row>
-    <row r="17" spans="1:44">
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
+      <c r="AU16" s="2"/>
+      <c r="AV16" s="2"/>
+      <c r="AW16" s="2"/>
+    </row>
+    <row r="17" spans="1:49">
       <c r="A17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1691,8 +1852,8 @@
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1725,8 +1886,13 @@
       <c r="AP17" s="2"/>
       <c r="AQ17" s="2"/>
       <c r="AR17" s="2"/>
-    </row>
-    <row r="18" spans="1:44">
+      <c r="AS17" s="2"/>
+      <c r="AT17" s="2"/>
+      <c r="AU17" s="2"/>
+      <c r="AV17" s="2"/>
+      <c r="AW17" s="2"/>
+    </row>
+    <row r="18" spans="1:49">
       <c r="A18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1734,8 +1900,8 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1768,8 +1934,13 @@
       <c r="AP18" s="2"/>
       <c r="AQ18" s="2"/>
       <c r="AR18" s="2"/>
-    </row>
-    <row r="19" spans="1:44">
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
+      <c r="AV18" s="2"/>
+      <c r="AW18" s="2"/>
+    </row>
+    <row r="19" spans="1:49">
       <c r="A19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1777,8 +1948,8 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1811,8 +1982,13 @@
       <c r="AP19" s="2"/>
       <c r="AQ19" s="2"/>
       <c r="AR19" s="2"/>
-    </row>
-    <row r="20" spans="1:44">
+      <c r="AS19" s="2"/>
+      <c r="AT19" s="2"/>
+      <c r="AU19" s="2"/>
+      <c r="AV19" s="2"/>
+      <c r="AW19" s="2"/>
+    </row>
+    <row r="20" spans="1:49">
       <c r="A20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1820,8 +1996,8 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1854,8 +2030,13 @@
       <c r="AP20" s="2"/>
       <c r="AQ20" s="2"/>
       <c r="AR20" s="2"/>
-    </row>
-    <row r="21" spans="1:44">
+      <c r="AS20" s="2"/>
+      <c r="AT20" s="2"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+    </row>
+    <row r="21" spans="1:49">
       <c r="A21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1863,8 +2044,8 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -1897,8 +2078,13 @@
       <c r="AP21" s="2"/>
       <c r="AQ21" s="2"/>
       <c r="AR21" s="2"/>
-    </row>
-    <row r="22" spans="1:44">
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+    </row>
+    <row r="22" spans="1:49">
       <c r="A22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1906,8 +2092,8 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -1940,8 +2126,13 @@
       <c r="AP22" s="2"/>
       <c r="AQ22" s="2"/>
       <c r="AR22" s="2"/>
-    </row>
-    <row r="23" spans="1:44">
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+    </row>
+    <row r="23" spans="1:49">
       <c r="A23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1949,8 +2140,8 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1983,8 +2174,13 @@
       <c r="AP23" s="2"/>
       <c r="AQ23" s="2"/>
       <c r="AR23" s="2"/>
-    </row>
-    <row r="24" spans="1:44">
+      <c r="AS23" s="2"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+    </row>
+    <row r="24" spans="1:49">
       <c r="A24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1992,8 +2188,8 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -2026,8 +2222,13 @@
       <c r="AP24" s="2"/>
       <c r="AQ24" s="2"/>
       <c r="AR24" s="2"/>
-    </row>
-    <row r="25" spans="1:44">
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+    </row>
+    <row r="25" spans="1:49">
       <c r="A25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2035,8 +2236,8 @@
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -2069,8 +2270,13 @@
       <c r="AP25" s="2"/>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
-    </row>
-    <row r="26" spans="1:44">
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+    </row>
+    <row r="26" spans="1:49">
       <c r="A26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -2078,8 +2284,8 @@
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -2112,8 +2318,13 @@
       <c r="AP26" s="2"/>
       <c r="AQ26" s="2"/>
       <c r="AR26" s="2"/>
-    </row>
-    <row r="27" spans="1:44">
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+    </row>
+    <row r="27" spans="1:49">
       <c r="A27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2121,8 +2332,8 @@
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -2155,8 +2366,13 @@
       <c r="AP27" s="2"/>
       <c r="AQ27" s="2"/>
       <c r="AR27" s="2"/>
-    </row>
-    <row r="28" spans="1:44">
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="2"/>
+      <c r="AW27" s="2"/>
+    </row>
+    <row r="28" spans="1:49">
       <c r="A28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2164,8 +2380,8 @@
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -2198,8 +2414,13 @@
       <c r="AP28" s="2"/>
       <c r="AQ28" s="2"/>
       <c r="AR28" s="2"/>
-    </row>
-    <row r="29" spans="1:44">
+      <c r="AS28" s="2"/>
+      <c r="AT28" s="2"/>
+      <c r="AU28" s="2"/>
+      <c r="AV28" s="2"/>
+      <c r="AW28" s="2"/>
+    </row>
+    <row r="29" spans="1:49">
       <c r="A29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2207,8 +2428,8 @@
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -2241,8 +2462,13 @@
       <c r="AP29" s="2"/>
       <c r="AQ29" s="2"/>
       <c r="AR29" s="2"/>
-    </row>
-    <row r="30" spans="1:44">
+      <c r="AS29" s="2"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="2"/>
+      <c r="AW29" s="2"/>
+    </row>
+    <row r="30" spans="1:49">
       <c r="A30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2250,8 +2476,8 @@
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -2284,8 +2510,13 @@
       <c r="AP30" s="2"/>
       <c r="AQ30" s="2"/>
       <c r="AR30" s="2"/>
-    </row>
-    <row r="31" spans="1:44">
+      <c r="AS30" s="2"/>
+      <c r="AT30" s="2"/>
+      <c r="AU30" s="2"/>
+      <c r="AV30" s="2"/>
+      <c r="AW30" s="2"/>
+    </row>
+    <row r="31" spans="1:49">
       <c r="A31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2293,8 +2524,8 @@
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
       <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -2327,8 +2558,13 @@
       <c r="AP31" s="2"/>
       <c r="AQ31" s="2"/>
       <c r="AR31" s="2"/>
-    </row>
-    <row r="32" spans="1:44">
+      <c r="AS31" s="2"/>
+      <c r="AT31" s="2"/>
+      <c r="AU31" s="2"/>
+      <c r="AV31" s="2"/>
+      <c r="AW31" s="2"/>
+    </row>
+    <row r="32" spans="1:49">
       <c r="A32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -2336,8 +2572,8 @@
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -2370,8 +2606,13 @@
       <c r="AP32" s="2"/>
       <c r="AQ32" s="2"/>
       <c r="AR32" s="2"/>
-    </row>
-    <row r="33" spans="1:44">
+      <c r="AS32" s="2"/>
+      <c r="AT32" s="2"/>
+      <c r="AU32" s="2"/>
+      <c r="AV32" s="2"/>
+      <c r="AW32" s="2"/>
+    </row>
+    <row r="33" spans="1:49">
       <c r="A33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2379,8 +2620,8 @@
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -2413,8 +2654,13 @@
       <c r="AP33" s="2"/>
       <c r="AQ33" s="2"/>
       <c r="AR33" s="2"/>
-    </row>
-    <row r="34" spans="1:44">
+      <c r="AS33" s="2"/>
+      <c r="AT33" s="2"/>
+      <c r="AU33" s="2"/>
+      <c r="AV33" s="2"/>
+      <c r="AW33" s="2"/>
+    </row>
+    <row r="34" spans="1:49">
       <c r="A34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -2422,8 +2668,8 @@
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -2456,8 +2702,13 @@
       <c r="AP34" s="2"/>
       <c r="AQ34" s="2"/>
       <c r="AR34" s="2"/>
-    </row>
-    <row r="35" spans="1:44">
+      <c r="AS34" s="2"/>
+      <c r="AT34" s="2"/>
+      <c r="AU34" s="2"/>
+      <c r="AV34" s="2"/>
+      <c r="AW34" s="2"/>
+    </row>
+    <row r="35" spans="1:49">
       <c r="A35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2465,8 +2716,8 @@
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -2499,8 +2750,13 @@
       <c r="AP35" s="2"/>
       <c r="AQ35" s="2"/>
       <c r="AR35" s="2"/>
-    </row>
-    <row r="36" spans="1:44">
+      <c r="AS35" s="2"/>
+      <c r="AT35" s="2"/>
+      <c r="AU35" s="2"/>
+      <c r="AV35" s="2"/>
+      <c r="AW35" s="2"/>
+    </row>
+    <row r="36" spans="1:49">
       <c r="A36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2508,8 +2764,8 @@
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -2542,8 +2798,13 @@
       <c r="AP36" s="2"/>
       <c r="AQ36" s="2"/>
       <c r="AR36" s="2"/>
-    </row>
-    <row r="37" spans="1:44">
+      <c r="AS36" s="2"/>
+      <c r="AT36" s="2"/>
+      <c r="AU36" s="2"/>
+      <c r="AV36" s="2"/>
+      <c r="AW36" s="2"/>
+    </row>
+    <row r="37" spans="1:49">
       <c r="A37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2551,8 +2812,8 @@
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -2585,8 +2846,13 @@
       <c r="AP37" s="2"/>
       <c r="AQ37" s="2"/>
       <c r="AR37" s="2"/>
-    </row>
-    <row r="38" spans="1:44">
+      <c r="AS37" s="2"/>
+      <c r="AT37" s="2"/>
+      <c r="AU37" s="2"/>
+      <c r="AV37" s="2"/>
+      <c r="AW37" s="2"/>
+    </row>
+    <row r="38" spans="1:49">
       <c r="A38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2594,8 +2860,8 @@
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -2628,8 +2894,13 @@
       <c r="AP38" s="2"/>
       <c r="AQ38" s="2"/>
       <c r="AR38" s="2"/>
-    </row>
-    <row r="39" spans="1:44">
+      <c r="AS38" s="2"/>
+      <c r="AT38" s="2"/>
+      <c r="AU38" s="2"/>
+      <c r="AV38" s="2"/>
+      <c r="AW38" s="2"/>
+    </row>
+    <row r="39" spans="1:49">
       <c r="A39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2637,8 +2908,8 @@
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -2671,8 +2942,13 @@
       <c r="AP39" s="2"/>
       <c r="AQ39" s="2"/>
       <c r="AR39" s="2"/>
-    </row>
-    <row r="40" spans="1:44">
+      <c r="AS39" s="2"/>
+      <c r="AT39" s="2"/>
+      <c r="AU39" s="2"/>
+      <c r="AV39" s="2"/>
+      <c r="AW39" s="2"/>
+    </row>
+    <row r="40" spans="1:49">
       <c r="A40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2680,8 +2956,8 @@
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -2714,8 +2990,13 @@
       <c r="AP40" s="2"/>
       <c r="AQ40" s="2"/>
       <c r="AR40" s="2"/>
-    </row>
-    <row r="41" spans="1:44">
+      <c r="AS40" s="2"/>
+      <c r="AT40" s="2"/>
+      <c r="AU40" s="2"/>
+      <c r="AV40" s="2"/>
+      <c r="AW40" s="2"/>
+    </row>
+    <row r="41" spans="1:49">
       <c r="A41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2723,8 +3004,8 @@
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -2757,8 +3038,13 @@
       <c r="AP41" s="2"/>
       <c r="AQ41" s="2"/>
       <c r="AR41" s="2"/>
-    </row>
-    <row r="42" spans="1:44">
+      <c r="AS41" s="2"/>
+      <c r="AT41" s="2"/>
+      <c r="AU41" s="2"/>
+      <c r="AV41" s="2"/>
+      <c r="AW41" s="2"/>
+    </row>
+    <row r="42" spans="1:49">
       <c r="A42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2766,8 +3052,8 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -2800,8 +3086,13 @@
       <c r="AP42" s="2"/>
       <c r="AQ42" s="2"/>
       <c r="AR42" s="2"/>
-    </row>
-    <row r="43" spans="1:44">
+      <c r="AS42" s="2"/>
+      <c r="AT42" s="2"/>
+      <c r="AU42" s="2"/>
+      <c r="AV42" s="2"/>
+      <c r="AW42" s="2"/>
+    </row>
+    <row r="43" spans="1:49">
       <c r="A43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2809,8 +3100,8 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -2843,8 +3134,13 @@
       <c r="AP43" s="2"/>
       <c r="AQ43" s="2"/>
       <c r="AR43" s="2"/>
-    </row>
-    <row r="44" spans="1:44">
+      <c r="AS43" s="2"/>
+      <c r="AT43" s="2"/>
+      <c r="AU43" s="2"/>
+      <c r="AV43" s="2"/>
+      <c r="AW43" s="2"/>
+    </row>
+    <row r="44" spans="1:49">
       <c r="A44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2852,8 +3148,8 @@
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -2886,8 +3182,13 @@
       <c r="AP44" s="2"/>
       <c r="AQ44" s="2"/>
       <c r="AR44" s="2"/>
-    </row>
-    <row r="45" spans="1:44">
+      <c r="AS44" s="2"/>
+      <c r="AT44" s="2"/>
+      <c r="AU44" s="2"/>
+      <c r="AV44" s="2"/>
+      <c r="AW44" s="2"/>
+    </row>
+    <row r="45" spans="1:49">
       <c r="A45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2895,8 +3196,8 @@
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -2929,8 +3230,13 @@
       <c r="AP45" s="2"/>
       <c r="AQ45" s="2"/>
       <c r="AR45" s="2"/>
-    </row>
-    <row r="46" spans="1:44">
+      <c r="AS45" s="2"/>
+      <c r="AT45" s="2"/>
+      <c r="AU45" s="2"/>
+      <c r="AV45" s="2"/>
+      <c r="AW45" s="2"/>
+    </row>
+    <row r="46" spans="1:49">
       <c r="A46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2938,8 +3244,8 @@
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
       <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -2972,8 +3278,13 @@
       <c r="AP46" s="2"/>
       <c r="AQ46" s="2"/>
       <c r="AR46" s="2"/>
-    </row>
-    <row r="47" spans="1:44">
+      <c r="AS46" s="2"/>
+      <c r="AT46" s="2"/>
+      <c r="AU46" s="2"/>
+      <c r="AV46" s="2"/>
+      <c r="AW46" s="2"/>
+    </row>
+    <row r="47" spans="1:49">
       <c r="A47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2981,8 +3292,8 @@
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
       <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -3015,8 +3326,13 @@
       <c r="AP47" s="2"/>
       <c r="AQ47" s="2"/>
       <c r="AR47" s="2"/>
-    </row>
-    <row r="48" spans="1:44">
+      <c r="AS47" s="2"/>
+      <c r="AT47" s="2"/>
+      <c r="AU47" s="2"/>
+      <c r="AV47" s="2"/>
+      <c r="AW47" s="2"/>
+    </row>
+    <row r="48" spans="1:49">
       <c r="A48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -3024,8 +3340,8 @@
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
       <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -3058,8 +3374,13 @@
       <c r="AP48" s="2"/>
       <c r="AQ48" s="2"/>
       <c r="AR48" s="2"/>
-    </row>
-    <row r="49" spans="1:44">
+      <c r="AS48" s="2"/>
+      <c r="AT48" s="2"/>
+      <c r="AU48" s="2"/>
+      <c r="AV48" s="2"/>
+      <c r="AW48" s="2"/>
+    </row>
+    <row r="49" spans="1:49">
       <c r="A49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -3067,8 +3388,8 @@
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
       <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -3101,8 +3422,13 @@
       <c r="AP49" s="2"/>
       <c r="AQ49" s="2"/>
       <c r="AR49" s="2"/>
-    </row>
-    <row r="50" spans="1:44">
+      <c r="AS49" s="2"/>
+      <c r="AT49" s="2"/>
+      <c r="AU49" s="2"/>
+      <c r="AV49" s="2"/>
+      <c r="AW49" s="2"/>
+    </row>
+    <row r="50" spans="1:49">
       <c r="A50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -3110,8 +3436,8 @@
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
       <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -3144,8 +3470,13 @@
       <c r="AP50" s="2"/>
       <c r="AQ50" s="2"/>
       <c r="AR50" s="2"/>
-    </row>
-    <row r="51" spans="1:44">
+      <c r="AS50" s="2"/>
+      <c r="AT50" s="2"/>
+      <c r="AU50" s="2"/>
+      <c r="AV50" s="2"/>
+      <c r="AW50" s="2"/>
+    </row>
+    <row r="51" spans="1:49">
       <c r="A51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -3153,8 +3484,8 @@
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
       <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -3187,8 +3518,13 @@
       <c r="AP51" s="2"/>
       <c r="AQ51" s="2"/>
       <c r="AR51" s="2"/>
-    </row>
-    <row r="52" spans="1:44">
+      <c r="AS51" s="2"/>
+      <c r="AT51" s="2"/>
+      <c r="AU51" s="2"/>
+      <c r="AV51" s="2"/>
+      <c r="AW51" s="2"/>
+    </row>
+    <row r="52" spans="1:49">
       <c r="A52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -3196,8 +3532,8 @@
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
       <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -3230,8 +3566,13 @@
       <c r="AP52" s="2"/>
       <c r="AQ52" s="2"/>
       <c r="AR52" s="2"/>
-    </row>
-    <row r="53" spans="1:44">
+      <c r="AS52" s="2"/>
+      <c r="AT52" s="2"/>
+      <c r="AU52" s="2"/>
+      <c r="AV52" s="2"/>
+      <c r="AW52" s="2"/>
+    </row>
+    <row r="53" spans="1:49">
       <c r="A53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -3239,8 +3580,8 @@
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
       <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -3273,8 +3614,13 @@
       <c r="AP53" s="2"/>
       <c r="AQ53" s="2"/>
       <c r="AR53" s="2"/>
-    </row>
-    <row r="54" spans="1:44">
+      <c r="AS53" s="2"/>
+      <c r="AT53" s="2"/>
+      <c r="AU53" s="2"/>
+      <c r="AV53" s="2"/>
+      <c r="AW53" s="2"/>
+    </row>
+    <row r="54" spans="1:49">
       <c r="A54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -3282,8 +3628,8 @@
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
       <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -3316,8 +3662,13 @@
       <c r="AP54" s="2"/>
       <c r="AQ54" s="2"/>
       <c r="AR54" s="2"/>
-    </row>
-    <row r="55" spans="1:44">
+      <c r="AS54" s="2"/>
+      <c r="AT54" s="2"/>
+      <c r="AU54" s="2"/>
+      <c r="AV54" s="2"/>
+      <c r="AW54" s="2"/>
+    </row>
+    <row r="55" spans="1:49">
       <c r="A55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -3325,8 +3676,8 @@
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
       <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -3359,8 +3710,13 @@
       <c r="AP55" s="2"/>
       <c r="AQ55" s="2"/>
       <c r="AR55" s="2"/>
-    </row>
-    <row r="56" spans="1:44">
+      <c r="AS55" s="2"/>
+      <c r="AT55" s="2"/>
+      <c r="AU55" s="2"/>
+      <c r="AV55" s="2"/>
+      <c r="AW55" s="2"/>
+    </row>
+    <row r="56" spans="1:49">
       <c r="A56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -3368,8 +3724,8 @@
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -3402,8 +3758,13 @@
       <c r="AP56" s="2"/>
       <c r="AQ56" s="2"/>
       <c r="AR56" s="2"/>
-    </row>
-    <row r="57" spans="1:44">
+      <c r="AS56" s="2"/>
+      <c r="AT56" s="2"/>
+      <c r="AU56" s="2"/>
+      <c r="AV56" s="2"/>
+      <c r="AW56" s="2"/>
+    </row>
+    <row r="57" spans="1:49">
       <c r="A57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -3411,8 +3772,8 @@
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
       <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -3445,8 +3806,13 @@
       <c r="AP57" s="2"/>
       <c r="AQ57" s="2"/>
       <c r="AR57" s="2"/>
-    </row>
-    <row r="58" spans="1:44">
+      <c r="AS57" s="2"/>
+      <c r="AT57" s="2"/>
+      <c r="AU57" s="2"/>
+      <c r="AV57" s="2"/>
+      <c r="AW57" s="2"/>
+    </row>
+    <row r="58" spans="1:49">
       <c r="A58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -3454,8 +3820,8 @@
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
       <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -3488,8 +3854,13 @@
       <c r="AP58" s="2"/>
       <c r="AQ58" s="2"/>
       <c r="AR58" s="2"/>
-    </row>
-    <row r="59" spans="1:44">
+      <c r="AS58" s="2"/>
+      <c r="AT58" s="2"/>
+      <c r="AU58" s="2"/>
+      <c r="AV58" s="2"/>
+      <c r="AW58" s="2"/>
+    </row>
+    <row r="59" spans="1:49">
       <c r="A59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -3497,8 +3868,8 @@
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
       <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -3531,8 +3902,13 @@
       <c r="AP59" s="2"/>
       <c r="AQ59" s="2"/>
       <c r="AR59" s="2"/>
-    </row>
-    <row r="60" spans="1:44">
+      <c r="AS59" s="2"/>
+      <c r="AT59" s="2"/>
+      <c r="AU59" s="2"/>
+      <c r="AV59" s="2"/>
+      <c r="AW59" s="2"/>
+    </row>
+    <row r="60" spans="1:49">
       <c r="A60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -3540,8 +3916,8 @@
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
       <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -3574,8 +3950,13 @@
       <c r="AP60" s="2"/>
       <c r="AQ60" s="2"/>
       <c r="AR60" s="2"/>
-    </row>
-    <row r="61" spans="1:44">
+      <c r="AS60" s="2"/>
+      <c r="AT60" s="2"/>
+      <c r="AU60" s="2"/>
+      <c r="AV60" s="2"/>
+      <c r="AW60" s="2"/>
+    </row>
+    <row r="61" spans="1:49">
       <c r="A61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -3583,8 +3964,8 @@
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
       <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -3617,8 +3998,13 @@
       <c r="AP61" s="2"/>
       <c r="AQ61" s="2"/>
       <c r="AR61" s="2"/>
-    </row>
-    <row r="62" spans="1:44">
+      <c r="AS61" s="2"/>
+      <c r="AT61" s="2"/>
+      <c r="AU61" s="2"/>
+      <c r="AV61" s="2"/>
+      <c r="AW61" s="2"/>
+    </row>
+    <row r="62" spans="1:49">
       <c r="A62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -3626,8 +4012,8 @@
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
       <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -3660,8 +4046,13 @@
       <c r="AP62" s="2"/>
       <c r="AQ62" s="2"/>
       <c r="AR62" s="2"/>
-    </row>
-    <row r="63" spans="1:44">
+      <c r="AS62" s="2"/>
+      <c r="AT62" s="2"/>
+      <c r="AU62" s="2"/>
+      <c r="AV62" s="2"/>
+      <c r="AW62" s="2"/>
+    </row>
+    <row r="63" spans="1:49">
       <c r="A63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3669,8 +4060,8 @@
       <c r="H63" s="12"/>
       <c r="I63" s="12"/>
       <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -3703,8 +4094,13 @@
       <c r="AP63" s="2"/>
       <c r="AQ63" s="2"/>
       <c r="AR63" s="2"/>
-    </row>
-    <row r="64" spans="1:44">
+      <c r="AS63" s="2"/>
+      <c r="AT63" s="2"/>
+      <c r="AU63" s="2"/>
+      <c r="AV63" s="2"/>
+      <c r="AW63" s="2"/>
+    </row>
+    <row r="64" spans="1:49">
       <c r="A64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -3712,8 +4108,8 @@
       <c r="H64" s="12"/>
       <c r="I64" s="12"/>
       <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -3746,8 +4142,13 @@
       <c r="AP64" s="2"/>
       <c r="AQ64" s="2"/>
       <c r="AR64" s="2"/>
-    </row>
-    <row r="65" spans="1:44">
+      <c r="AS64" s="2"/>
+      <c r="AT64" s="2"/>
+      <c r="AU64" s="2"/>
+      <c r="AV64" s="2"/>
+      <c r="AW64" s="2"/>
+    </row>
+    <row r="65" spans="1:49">
       <c r="A65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -3755,8 +4156,8 @@
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
       <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -3789,8 +4190,13 @@
       <c r="AP65" s="2"/>
       <c r="AQ65" s="2"/>
       <c r="AR65" s="2"/>
-    </row>
-    <row r="66" spans="1:44">
+      <c r="AS65" s="2"/>
+      <c r="AT65" s="2"/>
+      <c r="AU65" s="2"/>
+      <c r="AV65" s="2"/>
+      <c r="AW65" s="2"/>
+    </row>
+    <row r="66" spans="1:49">
       <c r="A66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -3798,8 +4204,8 @@
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
       <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -3832,8 +4238,13 @@
       <c r="AP66" s="2"/>
       <c r="AQ66" s="2"/>
       <c r="AR66" s="2"/>
-    </row>
-    <row r="67" spans="1:44">
+      <c r="AS66" s="2"/>
+      <c r="AT66" s="2"/>
+      <c r="AU66" s="2"/>
+      <c r="AV66" s="2"/>
+      <c r="AW66" s="2"/>
+    </row>
+    <row r="67" spans="1:49">
       <c r="A67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -3841,8 +4252,8 @@
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
       <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="12"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -3875,8 +4286,13 @@
       <c r="AP67" s="2"/>
       <c r="AQ67" s="2"/>
       <c r="AR67" s="2"/>
-    </row>
-    <row r="68" spans="1:44">
+      <c r="AS67" s="2"/>
+      <c r="AT67" s="2"/>
+      <c r="AU67" s="2"/>
+      <c r="AV67" s="2"/>
+      <c r="AW67" s="2"/>
+    </row>
+    <row r="68" spans="1:49">
       <c r="A68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -3884,8 +4300,8 @@
       <c r="H68" s="12"/>
       <c r="I68" s="12"/>
       <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -3918,25 +4334,30 @@
       <c r="AP68" s="2"/>
       <c r="AQ68" s="2"/>
       <c r="AR68" s="2"/>
+      <c r="AS68" s="2"/>
+      <c r="AT68" s="2"/>
+      <c r="AU68" s="2"/>
+      <c r="AV68" s="2"/>
+      <c r="AW68" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576 P2:P1048576">
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576 P2:P1048576">
       <formula1>"0,1,2,3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1:R1048576 O2:O1048576 AA2:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:W1048576 T2:T1048576 AF2:AF1048576">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576 Q2:Q1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X1048576 V2:V1048576">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576 W2:W1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y1048576 AB2:AB1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576 X2:X1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z1048576 AC2:AC1048576">
       <formula1>"0,1,2,3,4,5,6,7,8"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2:AE1048576">
       <formula1>"0,1+,2+,3+"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -3944,6 +4365,10 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>"Mastectomy,Partial Mastectomy,Lumpectomy"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:L1048576">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>